<commit_message>
added test coral and disease area measurements
</commit_message>
<xml_diff>
--- a/Coral_disease_measurements.xlsx
+++ b/Coral_disease_measurements.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mike/Documents/GitHub/Rhino-Python-3D-Coral-Reefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA82F6D9-FDE4-DD4A-8AC4-21CD7375366D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D8F1C7-D9B8-6742-A7EA-26716534F403}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19960" windowHeight="20000" xr2:uid="{75F0AD61-3AEC-EA4F-A575-D38ED96EAE18}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP58_8.24.18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Object</t>
   </si>
@@ -46,14 +46,50 @@
   </si>
   <si>
     <t>Area in sq m</t>
+  </si>
+  <si>
+    <t>Object 1</t>
+  </si>
+  <si>
+    <t>Object 2</t>
+  </si>
+  <si>
+    <t>Object 3</t>
+  </si>
+  <si>
+    <t>Object 4</t>
+  </si>
+  <si>
+    <t>Object 5</t>
+  </si>
+  <si>
+    <t>Object 6</t>
+  </si>
+  <si>
+    <t>mortality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,14 +114,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,15 +437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB80C258-423A-3E43-A943-5798EF2533AB}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,33 +456,80 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <f>D2/100/100</f>
-        <v>5.4051768899999997E-4</v>
-      </c>
-      <c r="D2">
+      <c r="I2">
         <v>5.4051768899999999</v>
       </c>
+      <c r="J2">
+        <f>I2*100*100</f>
+        <v>54051.768900000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0.16218480199999999</v>
+      </c>
+      <c r="D3">
+        <v>1.70914707E-2</v>
+      </c>
+      <c r="E3">
+        <v>8.4372147800000005E-3</v>
+      </c>
+      <c r="F3">
+        <v>6.8554444700000003E-3</v>
+      </c>
+      <c r="G3">
+        <v>5.51765668E-3</v>
+      </c>
+      <c r="H3">
+        <v>3.5400709299999999E-3</v>
+      </c>
+      <c r="I3">
+        <f>SUM(C3:H3)</f>
+        <v>0.20362665956000001</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">I3*100*100</f>
+        <v>2036.2665956000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -447,11 +537,30 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>5.2167188499999996E-3</v>
+        <v>2.96883294E-3</v>
       </c>
       <c r="D4">
-        <f>C4*100*100</f>
-        <v>52.167188499999995</v>
+        <v>1.9285350499999999E-3</v>
+      </c>
+      <c r="E4">
+        <v>3.1935085199999999E-4</v>
+      </c>
+      <c r="I4">
+        <f>SUM(C4:H4)</f>
+        <v>5.2167188419999996E-3</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>52.167188420000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2">
+        <f>(J4/J3)</f>
+        <v>2.5619036590161504E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>